<commit_message>
adicionados novos metodos e refatoração do codigo
</commit_message>
<xml_diff>
--- a/perfilNovo.xlsx
+++ b/perfilNovo.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CQ67"/>
+  <dimension ref="A1:CR67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -913,6 +913,11 @@
           <t>Escreva algumas linhas sobre sua história e seus sonhos de vida.</t>
         </is>
       </c>
+      <c r="CR1" s="1" t="inlineStr">
+        <is>
+          <t>Empregos Tratados</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1334,6 +1339,11 @@
       <c r="CQ2" t="inlineStr">
         <is>
           <t>Quero me formar para conseguir ganhar bastante dinheiro trabalhando na área!</t>
+        </is>
+      </c>
+      <c r="CR2" t="inlineStr">
+        <is>
+          <t>compasso uol</t>
         </is>
       </c>
     </row>
@@ -1755,6 +1765,7 @@
           <t>Meu objetivo é aprender muito, conseguir experiência suficiente para trabalhar, e conseguir um bom emprego e sustentar minha família.</t>
         </is>
       </c>
+      <c r="CR3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -2162,6 +2173,7 @@
           <t>Meu maior objetivo é ter mais conhecimento sobre a área da tecnologia e desenvolver minha própria empresa</t>
         </is>
       </c>
+      <c r="CR4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -2569,6 +2581,7 @@
           <t>Meu maior objetivo é trabalhar na área da tecnologia e ganhar bem para sustentar minha família e viajar com os amigos!</t>
         </is>
       </c>
+      <c r="CR5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -3002,6 +3015,11 @@
       <c r="CQ6" t="inlineStr">
         <is>
           <t>Meu objetivo é concluir o curso</t>
+        </is>
+      </c>
+      <c r="CR6" t="inlineStr">
+        <is>
+          <t>fatec franca</t>
         </is>
       </c>
     </row>
@@ -3355,6 +3373,11 @@
           <t>Meu maior objetivo é adquirir o máximo de conhecimento o possível durante a minha jornada acadêmica, trabalhar também com a área escolhida no curso mas também com a minha vocação que é a tatuagem.</t>
         </is>
       </c>
+      <c r="CR7" t="inlineStr">
+        <is>
+          <t>fogo vivo</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -3776,6 +3799,11 @@
       <c r="CQ8" t="inlineStr">
         <is>
           <t>Meu sonho é trabalhar por conta desenvolvendo Softwares e sites para empresas tanto nacional quanto no exterior, e não ter uma carga horária de trabalho definida.</t>
+        </is>
+      </c>
+      <c r="CR8" t="inlineStr">
+        <is>
+          <t>instituto samaritano de ensino</t>
         </is>
       </c>
     </row>
@@ -4185,6 +4213,7 @@
           <t xml:space="preserve">Em 2020, minha irmã ingressou na área da tecnologia e me incentivou a estudar também, no começo eu não quis mas depois fui me interessando pela área, fiz a prova e passei na FATEC, estou amando o curso e meu objetivo é pegar o diploma e trabalhar em alguma empresa nacional ou internacional na área de desenvolvimento mobile.    </t>
         </is>
       </c>
+      <c r="CR9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -4612,6 +4641,7 @@
           <t>Meu sonho é me estabilizar financeiramente e estar perto de quem eu amo</t>
         </is>
       </c>
+      <c r="CR10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -5033,6 +5063,11 @@
       <c r="CQ11" t="inlineStr">
         <is>
           <t xml:space="preserve">Me formar no curso de ADS e conseguir um trabalho na área sendo bem remunerado para dar uma boa qualidade de vida para minha família </t>
+        </is>
+      </c>
+      <c r="CR11" t="inlineStr">
+        <is>
+          <t>motorista de aplicativo</t>
         </is>
       </c>
     </row>
@@ -5462,6 +5497,7 @@
           <t>Abrir minha própria empresa no exterior e viajar o mundo.</t>
         </is>
       </c>
+      <c r="CR12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -5869,6 +5905,7 @@
           <t>Meu maior objetivo é ter um diploma de ensino superior, para que eu possa trabalhar no meu emprego dos sonhos!"</t>
         </is>
       </c>
+      <c r="CR13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -6292,6 +6329,11 @@
           <t xml:space="preserve">Meu objetivo é ter um diploma pr conquistar um bom emprego </t>
         </is>
       </c>
+      <c r="CR14" t="inlineStr">
+        <is>
+          <t>sd3 empreendimentos</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -6731,6 +6773,11 @@
           <t>Meu objetivo é conseguir uma melhor colocação no mercado de trabalho e estabilidade financeira.</t>
         </is>
       </c>
+      <c r="CR15" t="inlineStr">
+        <is>
+          <t>carmen steffens</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -7166,6 +7213,11 @@
           <t>Meu maior objetivo é conseguir uma vaga de emprego</t>
         </is>
       </c>
+      <c r="CR16" t="inlineStr">
+        <is>
+          <t>delivery</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -7589,6 +7641,11 @@
           <t>Meu objetivo é obter conhecimento pra um trabalho com remuneração boa, ter meu próprio negócio e uma possibilidade de trabalho remoto.</t>
         </is>
       </c>
+      <c r="CR17" t="inlineStr">
+        <is>
+          <t>camari</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -8012,6 +8069,11 @@
           <t xml:space="preserve">Meu objeto é me formar e poder fazer intercâmbio </t>
         </is>
       </c>
+      <c r="CR18" t="inlineStr">
+        <is>
+          <t>magazine luiza</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -8433,6 +8495,11 @@
       <c r="CQ19" t="inlineStr">
         <is>
           <t xml:space="preserve">Buscar mais conhecimento para que possa crescer profissionalmente e dar uma boa qualidade de vida a minha família </t>
+        </is>
+      </c>
+      <c r="CR19" t="inlineStr">
+        <is>
+          <t>corebiz</t>
         </is>
       </c>
     </row>
@@ -8854,6 +8921,7 @@
           <t>Meu maior objetivo é obter um diploma de curso superior e ingressar na área de programação trabalhando em uma empresa privada.</t>
         </is>
       </c>
+      <c r="CR20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -9289,6 +9357,11 @@
           <t>Meu objetivo é obter o conhecimento necessário na faculdade, para que posteriormente possa conseguir um emprego e uma remuneração melhor do que a atual.</t>
         </is>
       </c>
+      <c r="CR21" t="inlineStr">
+        <is>
+          <t>ramazzoni</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -9722,6 +9795,11 @@
       <c r="CQ22" t="inlineStr">
         <is>
           <t>Meu sonho é ter um emprego bem remunerado onde eu possa ajudar minha família, e eventualmente morar no exterior.</t>
+        </is>
+      </c>
+      <c r="CR22" t="inlineStr">
+        <is>
+          <t>simon vergan</t>
         </is>
       </c>
     </row>
@@ -10143,6 +10221,7 @@
           <t>Trabalhar para o exterior</t>
         </is>
       </c>
+      <c r="CR23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -10562,6 +10641,7 @@
           <t>Meu sonho no momento é poder melhorar como pessoa, conseguir um bom trabalho e proporcionar conforto pras pessoas próximas a mim.</t>
         </is>
       </c>
+      <c r="CR24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -10981,6 +11061,7 @@
           <t>Ter uma vida tranquila e estável (financeira, saúde, etc.)</t>
         </is>
       </c>
+      <c r="CR25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -11402,6 +11483,11 @@
       <c r="CQ26" t="inlineStr">
         <is>
           <t xml:space="preserve">Meu objetivo é me formar e ter um bom emprego, dando a minha família uma boa condição de vida </t>
+        </is>
+      </c>
+      <c r="CR26" t="inlineStr">
+        <is>
+          <t>empresa contratante vs clothes  loja de roupa</t>
         </is>
       </c>
     </row>
@@ -11823,6 +11909,7 @@
           <t xml:space="preserve">Meu maior objetivo até um momento e terminar a faculdade é adquirir competência pra trabalhar na área, e eventualmente conseguir uma vaga de emprego no exterior e mudar para lá </t>
         </is>
       </c>
+      <c r="CR27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -12242,6 +12329,7 @@
           <t>Minha meta principal é ser graduado, possuir um trablaho que goste e tenha uma vida estável enquanto faço o que me deixa feliz comigo mesmo, além de certa parte disso for investido em hobbies.</t>
         </is>
       </c>
+      <c r="CR28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -12669,6 +12757,11 @@
           <t xml:space="preserve">Meu maior sonho é conseguir a oportunidade de trabalhar fora do país </t>
         </is>
       </c>
+      <c r="CR29" t="inlineStr">
+        <is>
+          <t>fran plus</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -13104,6 +13197,11 @@
           <t>Conseguir um emprego nessa área para conquistar minhas própria coisas</t>
         </is>
       </c>
+      <c r="CR30" t="inlineStr">
+        <is>
+          <t>prefeitura municipal de ipua</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -13525,6 +13623,11 @@
       <c r="CQ31" t="inlineStr">
         <is>
           <t xml:space="preserve">Conseguir mudar de vida, ter um diploma e arrumar um emprego na área </t>
+        </is>
+      </c>
+      <c r="CR31" t="inlineStr">
+        <is>
+          <t>mds industria de saltos fabrica de solados</t>
         </is>
       </c>
     </row>
@@ -13946,6 +14049,7 @@
           <t xml:space="preserve">Tenho família, então busco melhor qualificação e oportunidades no mercado de trabalho! </t>
         </is>
       </c>
+      <c r="CR32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -14365,6 +14469,7 @@
           <t xml:space="preserve">Ser economicamente independente, conhecer vários lugares do mundo trabalhando de forma autônoma e com liberdade de atuação na área que escolhi. </t>
         </is>
       </c>
+      <c r="CR33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -14772,6 +14877,7 @@
           <t>Meu maior objetivo é me formar em engenharia da computação e e morar no exterior.</t>
         </is>
       </c>
+      <c r="CR34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -15203,6 +15309,11 @@
           <t>prefiro não responder</t>
         </is>
       </c>
+      <c r="CR35" t="inlineStr">
+        <is>
+          <t>globant</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -15626,6 +15737,11 @@
           <t>Meu objetivo é alcançar esse tão sonhado diploma, juntamente obter o conhecimento máximo e se inserir nesta área futuramente.</t>
         </is>
       </c>
+      <c r="CR36" t="inlineStr">
+        <is>
+          <t>telepublico</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -16049,6 +16165,11 @@
           <t>Tenho como objetivo pessoal minha estabilidade financeira e uma boa qualidade de vida para minha esposa e filhos.</t>
         </is>
       </c>
+      <c r="CR37" t="inlineStr">
+        <is>
+          <t>esquadros indrustria e comercio ltda</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -16472,6 +16593,11 @@
           <t>Meu maior objetivo é conquistar uma oportunidade na área e assim me integrar ao mercado de trabalho, em especial, me estabelecer no mercado exterior de tecnologia.</t>
         </is>
       </c>
+      <c r="CR38" t="inlineStr">
+        <is>
+          <t>santa casa de franca</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -16905,6 +17031,11 @@
       <c r="CQ39" t="inlineStr">
         <is>
           <t>Meu sonho é me tornar um profissional competitivo no mercado, capaz de impactar positivamente o ambiente onde estou inserido e conquistar a auto realização pessoal.</t>
+        </is>
+      </c>
+      <c r="CR39" t="inlineStr">
+        <is>
+          <t>magazine luiza</t>
         </is>
       </c>
     </row>
@@ -17314,6 +17445,7 @@
           <t xml:space="preserve">Meu objetivo é conseguir um bom trabalho que eu possa trabalhar remotamente para que eu consiga trabalhar em qualquer lugar com internet </t>
         </is>
       </c>
+      <c r="CR40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -17757,6 +17889,11 @@
           <t>O meu objetivo é me qualificar continuamente e consequentemente ter melhores resultados em todas as áreas.</t>
         </is>
       </c>
+      <c r="CR41" t="inlineStr">
+        <is>
+          <t>esquadros</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -18192,6 +18329,11 @@
           <t>Meu maior objetivo atualmente é conseguir um emprego na área em que estou cursando e assim poder crescer e aprimorar meus conhecimentos.</t>
         </is>
       </c>
+      <c r="CR42" t="inlineStr">
+        <is>
+          <t>ajesp</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -18613,6 +18755,11 @@
       <c r="CQ43" t="inlineStr">
         <is>
           <t xml:space="preserve">Me formar e conseguir um bom trabalho </t>
+        </is>
+      </c>
+      <c r="CR43" t="inlineStr">
+        <is>
+          <t>planalto tintas</t>
         </is>
       </c>
     </row>
@@ -19034,6 +19181,7 @@
           <t>Meu maior objetivo é ter um diploma de ensino superior, para que eu possa trabalhar em um emprego bem remunerado para facilitar a realização dos meus desejos.</t>
         </is>
       </c>
+      <c r="CR44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -19469,6 +19617,11 @@
           <t>Desejo continuar aprendendo sempre de modo a potencializar as minhas competencias e obter destaque profissional</t>
         </is>
       </c>
+      <c r="CR45" t="inlineStr">
+        <is>
+          <t>carmen steffens</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -19890,6 +20043,11 @@
       <c r="CQ46" t="inlineStr">
         <is>
           <t>Meu objetivo é conseguir trabalhar na área de TI, seja nacionalmente ou internacionalmente, além de ter uma forte vontade de morar fora do país.</t>
+        </is>
+      </c>
+      <c r="CR46" t="inlineStr">
+        <is>
+          <t>carmen steffens</t>
         </is>
       </c>
     </row>
@@ -20299,6 +20457,7 @@
           <t xml:space="preserve">Quero ter um diploma da área e adquirir novas habilidades para me tornar um bom profissional </t>
         </is>
       </c>
+      <c r="CR47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -20730,6 +20889,11 @@
           <t xml:space="preserve">Proporcionar a minha família uma qualidade de vida melhor </t>
         </is>
       </c>
+      <c r="CR48" t="inlineStr">
+        <is>
+          <t>motorista de aplicativo</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -21151,6 +21315,11 @@
       <c r="CQ49" t="inlineStr">
         <is>
           <t>Sou de uma familia simples e tenho como objetivo conquistar uma vida melhor atraves dos estudos</t>
+        </is>
+      </c>
+      <c r="CR49" t="inlineStr">
+        <is>
+          <t>unesp</t>
         </is>
       </c>
     </row>
@@ -21572,6 +21741,7 @@
           <t>Meu maior objetivo é me formar na área do curso de ADS para conquistar um bom trabalho e ter qualidade de vida.</t>
         </is>
       </c>
+      <c r="CR50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -21995,6 +22165,11 @@
           <t>Tenho o sonho de alcançar minha estabilidade financeira e viver uma vida confortável.</t>
         </is>
       </c>
+      <c r="CR51" t="inlineStr">
+        <is>
+          <t>magazine luiza</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -22418,6 +22593,11 @@
           <t>Meu objetivo é ser um professor universitário na área de tecnologia</t>
         </is>
       </c>
+      <c r="CR52" t="inlineStr">
+        <is>
+          <t>prefeitura municipal de sales oliveira</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -22851,6 +23031,11 @@
       <c r="CQ53" t="inlineStr">
         <is>
           <t>Já tenho um diploma de ensino superior, sou feliz com o que faço atualmente não me sinto valorizado pela sociedade. Sempre me interessei desde criança por tecnologia, videogames, computadores… Os avancos tecnológicos me encantam.</t>
+        </is>
+      </c>
+      <c r="CR53" t="inlineStr">
+        <is>
+          <t>estado de minas gerais</t>
         </is>
       </c>
     </row>
@@ -23272,6 +23457,7 @@
           <t>Meu objetivo é ter uma vida com grande liberdade financeira.</t>
         </is>
       </c>
+      <c r="CR54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -23695,6 +23881,11 @@
           <t>Tenho objetivo de ter uma melhor condição financeira e melhora minha qualidade de vida</t>
         </is>
       </c>
+      <c r="CR55" t="inlineStr">
+        <is>
+          <t>magazine luiza</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -24130,6 +24321,11 @@
           <t>Meu maior sonho no momento é poder proporcionar uma vida melhor para a minha família.</t>
         </is>
       </c>
+      <c r="CR56" t="inlineStr">
+        <is>
+          <t>secretaria estadual de educacao de sao paulo</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -24565,6 +24761,11 @@
           <t>Meu objetivo é conquistar o diploma de ensino superior para iniciar profissionalmente na área e conseguir uma estabilidade financeira e levar minha família junto comigo rumo ao sucesso</t>
         </is>
       </c>
+      <c r="CR57" t="inlineStr">
+        <is>
+          <t>jussara</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -25000,6 +25201,11 @@
           <t>Moro em Pedregulho, tenho conhecimento intermediário na área de tecnologia, meu objetivo é me formar e conquistar um emprego na área</t>
         </is>
       </c>
+      <c r="CR58" t="inlineStr">
+        <is>
+          <t>fimm</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -25435,6 +25641,11 @@
           <t>Meu maior objetivo é me especializar na área de tecnologia para aplicar esses conhecimentos juntamente com minha experiencia na área de saúde, a qual atuo no presente momento.</t>
         </is>
       </c>
+      <c r="CR59" t="inlineStr">
+        <is>
+          <t>atemoh</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -25870,6 +26081,11 @@
           <t>Meu maior objetivo de vida é me desenvolver como pessoa, tendo melhores relacionamentos e construindo uma vida ética e de sucesso.</t>
         </is>
       </c>
+      <c r="CR60" t="inlineStr">
+        <is>
+          <t>secretaria de transporte</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -26293,6 +26509,11 @@
           <t xml:space="preserve">Meu objetivo é ter um emprego bem remunerado e futuramente começar a dar aula em alguma faculdade </t>
         </is>
       </c>
+      <c r="CR61" t="inlineStr">
+        <is>
+          <t>irmao patrocinio</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -26728,6 +26949,11 @@
           <t>Utilizar conhecimentos da ADS como TDICs na Educação ou aplicar os conhecimentos no setor produtivo.</t>
         </is>
       </c>
+      <c r="CR62" t="inlineStr">
+        <is>
+          <t>escola estadual</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -27151,6 +27377,11 @@
           <t>Meu maior objetivo é fazer parte de cargo de gerencia e também, me tornar empresária.</t>
         </is>
       </c>
+      <c r="CR63" t="inlineStr">
+        <is>
+          <t>corebiz</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -27582,6 +27813,11 @@
           <t xml:space="preserve">Ser assalariado </t>
         </is>
       </c>
+      <c r="CR64" t="inlineStr">
+        <is>
+          <t>yares</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -28009,6 +28245,11 @@
           <t xml:space="preserve">Gostaria de terminar a faculdade para ter uma situação financeira tranquila </t>
         </is>
       </c>
+      <c r="CR65" t="inlineStr">
+        <is>
+          <t>master racing franca</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -28432,6 +28673,11 @@
           <t>Meu maior objetivo é comprar uma casa e ter um bom salário e dar uma boa condição para o meu pai.</t>
         </is>
       </c>
+      <c r="CR66" t="inlineStr">
+        <is>
+          <t>hortifruti da terra</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -28853,6 +29099,11 @@
       <c r="CQ67" t="inlineStr">
         <is>
           <t>Meu objetivo é concluir o curso e trabalhar em uma nova área, adquirir experiência na área</t>
+        </is>
+      </c>
+      <c r="CR67" t="inlineStr">
+        <is>
+          <t>secretaria do estado de sao paulo</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix alguns erros de digitação
</commit_message>
<xml_diff>
--- a/perfilNovo.xlsx
+++ b/perfilNovo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CO67"/>
+  <dimension ref="A1:CP67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -891,6 +891,11 @@
       </c>
       <c r="CO1" s="1" t="inlineStr">
         <is>
+          <t>Faixa Etária</t>
+        </is>
+      </c>
+      <c r="CP1" s="1" t="inlineStr">
+        <is>
           <t>Sonhos mais recorrentes</t>
         </is>
       </c>
@@ -1311,6 +1316,11 @@
         </is>
       </c>
       <c r="CO2" t="inlineStr">
+        <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP2" t="inlineStr">
         <is>
           <t>ganhar bastante dinheiro</t>
         </is>
@@ -1725,6 +1735,11 @@
       <c r="CN3" t="inlineStr"/>
       <c r="CO3" t="inlineStr">
         <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP3" t="inlineStr">
+        <is>
           <t>ganhar bastante dinheiro</t>
         </is>
       </c>
@@ -2126,6 +2141,11 @@
       <c r="CN4" t="inlineStr"/>
       <c r="CO4" t="inlineStr">
         <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP4" t="inlineStr">
+        <is>
           <t>conseguir experiência</t>
         </is>
       </c>
@@ -2527,6 +2547,11 @@
       <c r="CN5" t="inlineStr"/>
       <c r="CO5" t="inlineStr">
         <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP5" t="inlineStr">
+        <is>
           <t>conseguir um bom emprego</t>
         </is>
       </c>
@@ -2959,6 +2984,11 @@
         </is>
       </c>
       <c r="CO6" t="inlineStr">
+        <is>
+          <t>entre 30 e 35</t>
+        </is>
+      </c>
+      <c r="CP6" t="inlineStr">
         <is>
           <t>desenvolver minha própria empresa</t>
         </is>
@@ -3309,6 +3339,11 @@
       </c>
       <c r="CO7" t="inlineStr">
         <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP7" t="inlineStr">
+        <is>
           <t>trabalhar na área</t>
         </is>
       </c>
@@ -3729,6 +3764,11 @@
         </is>
       </c>
       <c r="CO8" t="inlineStr">
+        <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP8" t="inlineStr">
         <is>
           <t>viajar com os amigos</t>
         </is>
@@ -4131,6 +4171,11 @@
       <c r="CN9" t="inlineStr"/>
       <c r="CO9" t="inlineStr">
         <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP9" t="inlineStr">
+        <is>
           <t>adquirir o máximo</t>
         </is>
       </c>
@@ -4552,6 +4597,11 @@
       <c r="CN10" t="inlineStr"/>
       <c r="CO10" t="inlineStr">
         <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP10" t="inlineStr">
+        <is>
           <t>trabalhar por conta</t>
         </is>
       </c>
@@ -4972,6 +5022,11 @@
         </is>
       </c>
       <c r="CO11" t="inlineStr">
+        <is>
+          <t>entre 25 e 30</t>
+        </is>
+      </c>
+      <c r="CP11" t="inlineStr">
         <is>
           <t>trabalhar em alguma empresa</t>
         </is>
@@ -5394,6 +5449,11 @@
       <c r="CN12" t="inlineStr"/>
       <c r="CO12" t="inlineStr">
         <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP12" t="inlineStr">
+        <is>
           <t>conseguir um trabalho</t>
         </is>
       </c>
@@ -5795,6 +5855,11 @@
       <c r="CN13" t="inlineStr"/>
       <c r="CO13" t="inlineStr">
         <is>
+          <t>entre 30 e 35</t>
+        </is>
+      </c>
+      <c r="CP13" t="inlineStr">
+        <is>
           <t>viajar o mundo</t>
         </is>
       </c>
@@ -6216,6 +6281,11 @@
       </c>
       <c r="CO14" t="inlineStr">
         <is>
+          <t>entre 35 e 40</t>
+        </is>
+      </c>
+      <c r="CP14" t="inlineStr">
+        <is>
           <t>trabalhar no meu emprego</t>
         </is>
       </c>
@@ -6653,6 +6723,11 @@
       </c>
       <c r="CO15" t="inlineStr">
         <is>
+          <t>entre 35 e 40</t>
+        </is>
+      </c>
+      <c r="CP15" t="inlineStr">
+        <is>
           <t>conseguir um bom emprego</t>
         </is>
       </c>
@@ -7086,6 +7161,11 @@
       </c>
       <c r="CO16" t="inlineStr">
         <is>
+          <t>Acima de 40</t>
+        </is>
+      </c>
+      <c r="CP16" t="inlineStr">
+        <is>
           <t>conseguir uma melhor colocação</t>
         </is>
       </c>
@@ -7507,6 +7587,11 @@
       </c>
       <c r="CO17" t="inlineStr">
         <is>
+          <t>entre 30 e 35</t>
+        </is>
+      </c>
+      <c r="CP17" t="inlineStr">
+        <is>
           <t>conseguir uma vaga</t>
         </is>
       </c>
@@ -7928,6 +8013,11 @@
       </c>
       <c r="CO18" t="inlineStr">
         <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP18" t="inlineStr">
+        <is>
           <t>obter conhecimento</t>
         </is>
       </c>
@@ -8348,6 +8438,11 @@
         </is>
       </c>
       <c r="CO19" t="inlineStr">
+        <is>
+          <t>entre 25 e 30</t>
+        </is>
+      </c>
+      <c r="CP19" t="inlineStr">
         <is>
           <t>obter um diploma</t>
         </is>
@@ -8762,6 +8857,11 @@
       <c r="CN20" t="inlineStr"/>
       <c r="CO20" t="inlineStr">
         <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP20" t="inlineStr">
+        <is>
           <t>obter conhecimento</t>
         </is>
       </c>
@@ -9195,6 +9295,11 @@
       </c>
       <c r="CO21" t="inlineStr">
         <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP21" t="inlineStr">
+        <is>
           <t>conseguir um bom emprego</t>
         </is>
       </c>
@@ -9627,6 +9732,11 @@
         </is>
       </c>
       <c r="CO22" t="inlineStr">
+        <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP22" t="inlineStr">
         <is>
           <t>trabalhar para o exterior</t>
         </is>
@@ -10041,6 +10151,11 @@
       <c r="CN23" t="inlineStr"/>
       <c r="CO23" t="inlineStr">
         <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP23" t="inlineStr">
+        <is>
           <t>conseguir um trabalho</t>
         </is>
       </c>
@@ -10454,6 +10569,11 @@
       <c r="CN24" t="inlineStr"/>
       <c r="CO24" t="inlineStr">
         <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP24" t="inlineStr">
+        <is>
           <t>adquirir competência</t>
         </is>
       </c>
@@ -10867,6 +10987,11 @@
       <c r="CN25" t="inlineStr"/>
       <c r="CO25" t="inlineStr">
         <is>
+          <t>entre 25 e 30</t>
+        </is>
+      </c>
+      <c r="CP25" t="inlineStr">
+        <is>
           <t>trabalhar na área</t>
         </is>
       </c>
@@ -11287,6 +11412,11 @@
         </is>
       </c>
       <c r="CO26" t="inlineStr">
+        <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP26" t="inlineStr">
         <is>
           <t>conseguir uma vaga</t>
         </is>
@@ -11701,6 +11831,11 @@
       <c r="CN27" t="inlineStr"/>
       <c r="CO27" t="inlineStr">
         <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP27" t="inlineStr">
+        <is>
           <t>conseguir a oportunidade</t>
         </is>
       </c>
@@ -12114,6 +12249,11 @@
       <c r="CN28" t="inlineStr"/>
       <c r="CO28" t="inlineStr">
         <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP28" t="inlineStr">
+        <is>
           <t>trabalhar fora do país</t>
         </is>
       </c>
@@ -12539,6 +12679,11 @@
       </c>
       <c r="CO29" t="inlineStr">
         <is>
+          <t>entre 25 e 30</t>
+        </is>
+      </c>
+      <c r="CP29" t="inlineStr">
+        <is>
           <t>conseguir um bom emprego</t>
         </is>
       </c>
@@ -12972,6 +13117,11 @@
       </c>
       <c r="CO30" t="inlineStr">
         <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP30" t="inlineStr">
+        <is>
           <t>conquistar minhas própria coisas</t>
         </is>
       </c>
@@ -13392,6 +13542,11 @@
         </is>
       </c>
       <c r="CO31" t="inlineStr">
+        <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP31" t="inlineStr">
         <is>
           <t>mudar de vida</t>
         </is>
@@ -13806,6 +13961,11 @@
       <c r="CN32" t="inlineStr"/>
       <c r="CO32" t="inlineStr">
         <is>
+          <t>entre 30 e 35</t>
+        </is>
+      </c>
+      <c r="CP32" t="inlineStr">
+        <is>
           <t>conseguir mudar de vida</t>
         </is>
       </c>
@@ -14219,6 +14379,11 @@
       <c r="CN33" t="inlineStr"/>
       <c r="CO33" t="inlineStr">
         <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP33" t="inlineStr">
+        <is>
           <t>conhecer vários lugares</t>
         </is>
       </c>
@@ -14620,6 +14785,11 @@
       <c r="CN34" t="inlineStr"/>
       <c r="CO34" t="inlineStr">
         <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP34" t="inlineStr">
+        <is>
           <t>obter conhecimento</t>
         </is>
       </c>
@@ -15049,6 +15219,11 @@
       </c>
       <c r="CO35" t="inlineStr">
         <is>
+          <t>entre 30 e 35</t>
+        </is>
+      </c>
+      <c r="CP35" t="inlineStr">
+        <is>
           <t>conseguir a oportunidade</t>
         </is>
       </c>
@@ -15470,6 +15645,11 @@
       </c>
       <c r="CO36" t="inlineStr">
         <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP36" t="inlineStr">
+        <is>
           <t>conquistar a auto</t>
         </is>
       </c>
@@ -15891,6 +16071,11 @@
       </c>
       <c r="CO37" t="inlineStr">
         <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP37" t="inlineStr">
+        <is>
           <t>conquistar a auto realização</t>
         </is>
       </c>
@@ -16312,6 +16497,11 @@
       </c>
       <c r="CO38" t="inlineStr">
         <is>
+          <t>entre 30 e 35</t>
+        </is>
+      </c>
+      <c r="CP38" t="inlineStr">
+        <is>
           <t>conseguir um trabalho</t>
         </is>
       </c>
@@ -16744,6 +16934,11 @@
         </is>
       </c>
       <c r="CO39" t="inlineStr">
+        <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP39" t="inlineStr">
         <is>
           <t>trabalhar em qualquer lugar</t>
         </is>
@@ -17146,6 +17341,11 @@
       <c r="CN40" t="inlineStr"/>
       <c r="CO40" t="inlineStr">
         <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP40" t="inlineStr">
+        <is>
           <t>conseguir um bom emprego</t>
         </is>
       </c>
@@ -17587,6 +17787,11 @@
       </c>
       <c r="CO41" t="inlineStr">
         <is>
+          <t>entre 35 e 40</t>
+        </is>
+      </c>
+      <c r="CP41" t="inlineStr">
+        <is>
           <t>conseguir um trabalho</t>
         </is>
       </c>
@@ -18020,6 +18225,11 @@
       </c>
       <c r="CO42" t="inlineStr">
         <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP42" t="inlineStr">
+        <is>
           <t>trabalhar em alguma empresa</t>
         </is>
       </c>
@@ -18440,6 +18650,11 @@
         </is>
       </c>
       <c r="CO43" t="inlineStr">
+        <is>
+          <t>entre 30 e 35</t>
+        </is>
+      </c>
+      <c r="CP43" t="inlineStr">
         <is>
           <t>obter destaque</t>
         </is>
@@ -18854,6 +19069,11 @@
       <c r="CN44" t="inlineStr"/>
       <c r="CO44" t="inlineStr">
         <is>
+          <t>entre 30 e 35</t>
+        </is>
+      </c>
+      <c r="CP44" t="inlineStr">
+        <is>
           <t>trabalhar na área</t>
         </is>
       </c>
@@ -19287,6 +19507,11 @@
       </c>
       <c r="CO45" t="inlineStr">
         <is>
+          <t>entre 35 e 40</t>
+        </is>
+      </c>
+      <c r="CP45" t="inlineStr">
+        <is>
           <t>conseguir trabalhar na área</t>
         </is>
       </c>
@@ -19707,6 +19932,11 @@
         </is>
       </c>
       <c r="CO46" t="inlineStr">
+        <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP46" t="inlineStr">
         <is>
           <t>adquirir novas habilidades</t>
         </is>
@@ -20109,6 +20339,11 @@
       <c r="CN47" t="inlineStr"/>
       <c r="CO47" t="inlineStr">
         <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP47" t="inlineStr">
+        <is>
           <t>conquistar uma vida</t>
         </is>
       </c>
@@ -20538,6 +20773,11 @@
       </c>
       <c r="CO48" t="inlineStr">
         <is>
+          <t>entre 35 e 40</t>
+        </is>
+      </c>
+      <c r="CP48" t="inlineStr">
+        <is>
           <t>conseguir um bom trabalho</t>
         </is>
       </c>
@@ -20958,6 +21198,11 @@
         </is>
       </c>
       <c r="CO49" t="inlineStr">
+        <is>
+          <t>entre 30 e 35</t>
+        </is>
+      </c>
+      <c r="CP49" t="inlineStr">
         <is>
           <t>ser um professor</t>
         </is>
@@ -21372,6 +21617,11 @@
       <c r="CN50" t="inlineStr"/>
       <c r="CO50" t="inlineStr">
         <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP50" t="inlineStr">
+        <is>
           <t>conquistar o diploma</t>
         </is>
       </c>
@@ -21793,6 +22043,11 @@
       </c>
       <c r="CO51" t="inlineStr">
         <is>
+          <t>entre 30 e 35</t>
+        </is>
+      </c>
+      <c r="CP51" t="inlineStr">
+        <is>
           <t>conseguir uma estabilidade</t>
         </is>
       </c>
@@ -22214,6 +22469,11 @@
       </c>
       <c r="CO52" t="inlineStr">
         <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP52" t="inlineStr">
+        <is>
           <t>conquistar um bom emprego</t>
         </is>
       </c>
@@ -22646,6 +22906,11 @@
         </is>
       </c>
       <c r="CO53" t="inlineStr">
+        <is>
+          <t>entre 30 e 35</t>
+        </is>
+      </c>
+      <c r="CP53" t="inlineStr">
         <is>
           <t>desenvolver como pessoa</t>
         </is>
@@ -23060,6 +23325,11 @@
       <c r="CN54" t="inlineStr"/>
       <c r="CO54" t="inlineStr">
         <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP54" t="inlineStr">
+        <is>
           <t>adquirir experiência</t>
         </is>
       </c>
@@ -23481,6 +23751,11 @@
       </c>
       <c r="CO55" t="inlineStr">
         <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP55" t="inlineStr">
+        <is>
           <t>adquirir experiência</t>
         </is>
       </c>
@@ -23912,7 +24187,12 @@
           <t>secretaria estadual de educacao de sao paulo</t>
         </is>
       </c>
-      <c r="CO56" t="inlineStr"/>
+      <c r="CO56" t="inlineStr">
+        <is>
+          <t>Acima de 40</t>
+        </is>
+      </c>
+      <c r="CP56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -24341,7 +24621,12 @@
           <t>jussara</t>
         </is>
       </c>
-      <c r="CO57" t="inlineStr"/>
+      <c r="CO57" t="inlineStr">
+        <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -24770,7 +25055,12 @@
           <t>fimm</t>
         </is>
       </c>
-      <c r="CO58" t="inlineStr"/>
+      <c r="CO58" t="inlineStr">
+        <is>
+          <t>entre 20 e 25</t>
+        </is>
+      </c>
+      <c r="CP58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -25199,7 +25489,12 @@
           <t>atemoh</t>
         </is>
       </c>
-      <c r="CO59" t="inlineStr"/>
+      <c r="CO59" t="inlineStr">
+        <is>
+          <t>entre 30 e 35</t>
+        </is>
+      </c>
+      <c r="CP59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -25628,7 +25923,12 @@
           <t>secretaria de transporte</t>
         </is>
       </c>
-      <c r="CO60" t="inlineStr"/>
+      <c r="CO60" t="inlineStr">
+        <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -26045,7 +26345,12 @@
           <t>irmao patrocinio</t>
         </is>
       </c>
-      <c r="CO61" t="inlineStr"/>
+      <c r="CO61" t="inlineStr">
+        <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -26474,7 +26779,12 @@
           <t>escola estadual</t>
         </is>
       </c>
-      <c r="CO62" t="inlineStr"/>
+      <c r="CO62" t="inlineStr">
+        <is>
+          <t>Acima de 40</t>
+        </is>
+      </c>
+      <c r="CP62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -26891,7 +27201,12 @@
           <t>corebiz</t>
         </is>
       </c>
-      <c r="CO63" t="inlineStr"/>
+      <c r="CO63" t="inlineStr">
+        <is>
+          <t>entre 25 e 30</t>
+        </is>
+      </c>
+      <c r="CP63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -27316,7 +27631,12 @@
           <t>yares</t>
         </is>
       </c>
-      <c r="CO64" t="inlineStr"/>
+      <c r="CO64" t="inlineStr">
+        <is>
+          <t>entre 25 e 30</t>
+        </is>
+      </c>
+      <c r="CP64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -27737,7 +28057,12 @@
           <t>master racing franca</t>
         </is>
       </c>
-      <c r="CO65" t="inlineStr"/>
+      <c r="CO65" t="inlineStr">
+        <is>
+          <t>entre 25 e 30</t>
+        </is>
+      </c>
+      <c r="CP65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -28154,7 +28479,12 @@
           <t>hortifruti da terra</t>
         </is>
       </c>
-      <c r="CO66" t="inlineStr"/>
+      <c r="CO66" t="inlineStr">
+        <is>
+          <t>Entre 15 e 20</t>
+        </is>
+      </c>
+      <c r="CP66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -28571,7 +28901,12 @@
           <t>secretaria do estado de sao paulo</t>
         </is>
       </c>
-      <c r="CO67" t="inlineStr"/>
+      <c r="CO67" t="inlineStr">
+        <is>
+          <t>entre 30 e 35</t>
+        </is>
+      </c>
+      <c r="CP67" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>